<commit_message>
SollWert für alle Modelle
</commit_message>
<xml_diff>
--- a/Datasheets/DSOX6004A.xlsx
+++ b/Datasheets/DSOX6004A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3cb3f6eeceb65200/Documents/Albstadt/5Semester/Extraktion_aus_Datenblättern_mit_KI/Projekt_Extraktion/Datasheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_11C9E8F28FAAC3E2ADAAF6CD1680CB395430159B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{898E1A62-9058-4542-8A17-365F46387663}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="11_11C9E8F28FAAC3E2ADAAF6CD1680CB395430159B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{766AF72D-4325-4B6B-BF95-41B6E7B58F02}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="26160" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t>Versuch</t>
   </si>
@@ -387,6 +387,23 @@
   }
 }</t>
   </si>
+  <si>
+    <t>Zone (hardware zone qualifier), Edge, Edge then edge (B trigger), Pulse width, Pattern, Or, Rise/fall time, Nth edge burst, Runt, Setup and hold, Video
+Optional: Enhanced video</t>
+  </si>
+  <si>
+    <t>Touchscreen</t>
+  </si>
+  <si>
+    <t>USB, LAN</t>
+  </si>
+  <si>
+    <t>Optional: ARINC429, CAN, FlexRay, I²C, I²S, LIN, MIL-STD1553, SPI, UART/RS232/422/485, USB, SENT, User-definable Manchester/NRZ, CXPI, USB PD</t>
+  </si>
+  <si>
+    <t>Bandbreitenupgrade nachträglich möglich
+Optional: Enhanced Security</t>
+  </si>
 </sst>
 </file>
 
@@ -436,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -444,6 +461,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -790,7 +816,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -810,36 +838,57 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B3">
+        <v>1000</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -850,80 +899,128 @@
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B10">
+        <v>30.7</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>450000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -936,7 +1033,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,9 +1061,9 @@
         <f>Target_Values!A2</f>
         <v>Modell</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="1" t="str">
         <f>Target_Values!B2</f>
-        <v>0</v>
+        <v>DSOX6004A</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>26</v>
@@ -980,7 +1077,7 @@
       </c>
       <c r="B3" s="1">
         <f>Target_Values!B3</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>27</v>
@@ -994,7 +1091,7 @@
       </c>
       <c r="B4" s="1">
         <f>Target_Values!B4</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2">
         <v>4</v>
@@ -1008,7 +1105,7 @@
       </c>
       <c r="B5" s="1">
         <f>Target_Values!B5</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2">
         <v>20</v>
@@ -1022,7 +1119,7 @@
       </c>
       <c r="B6" s="1">
         <f>Target_Values!B6</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2">
         <v>4</v>
@@ -1034,9 +1131,10 @@
         <f>Target_Values!A7</f>
         <v>Triggerarten</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="6" t="str">
         <f>Target_Values!B7</f>
-        <v>0</v>
+        <v>Zone (hardware zone qualifier), Edge, Edge then edge (B trigger), Pulse width, Pattern, Or, Rise/fall time, Nth edge burst, Runt, Setup and hold, Video
+Optional: Enhanced video</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>28</v>
@@ -1050,7 +1148,7 @@
       </c>
       <c r="B8" s="1">
         <f>Target_Values!B8</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2">
         <v>8</v>
@@ -1078,7 +1176,7 @@
       </c>
       <c r="B10" s="1">
         <f>Target_Values!B10</f>
-        <v>0</v>
+        <v>30.7</v>
       </c>
       <c r="C10" s="2">
         <v>30.73</v>
@@ -1090,25 +1188,25 @@
         <f>Target_Values!A11</f>
         <v>Bildschirmtyp.pixel</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="1" t="str">
         <f>Target_Values!B11</f>
-        <v>0</v>
+        <v>800, 600</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="str">
         <f>Target_Values!A12</f>
         <v>Bildschirmtyp.screen_type</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="1" t="str">
         <f>Target_Values!B12</f>
-        <v>0</v>
-      </c>
-      <c r="C12" s="2" t="s">
+        <v>Touchscreen</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D12" s="2"/>
@@ -1118,9 +1216,9 @@
         <f>Target_Values!A13</f>
         <v>Schnittstellen.relevant_interfaces</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="1" t="str">
         <f>Target_Values!B13</f>
-        <v>0</v>
+        <v>USB, LAN</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>31</v>
@@ -1132,9 +1230,9 @@
         <f>Target_Values!A14</f>
         <v>Schnittstellen.optionale_interfaces</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="1" t="str">
         <f>Target_Values!B14</f>
-        <v>0</v>
+        <v>GPIB</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>32</v>
@@ -1146,9 +1244,9 @@
         <f>Target_Values!A15</f>
         <v>unterstützende serielle Busse</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="1" t="str">
         <f>Target_Values!B15</f>
-        <v>0</v>
+        <v>Optional: ARINC429, CAN, FlexRay, I²C, I²S, LIN, MIL-STD1553, SPI, UART/RS232/422/485, USB, SENT, User-definable Manchester/NRZ, CXPI, USB PD</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>33</v>
@@ -1162,7 +1260,7 @@
       </c>
       <c r="B16" s="1">
         <f>Target_Values!B16</f>
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="C16" s="2">
         <v>450000</v>
@@ -1174,9 +1272,9 @@
         <f>Target_Values!A17</f>
         <v>segmentierbarer Speicher</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="1" t="str">
         <f>Target_Values!B17</f>
-        <v>0</v>
+        <v>Yes</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>34</v>
@@ -1188,9 +1286,9 @@
         <f>Target_Values!A18</f>
         <v>Funktionsgenerator</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="1" t="str">
         <f>Target_Values!B18</f>
-        <v>0</v>
+        <v>Optional</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>35</v>
@@ -1202,9 +1300,9 @@
         <f>Target_Values!A19</f>
         <v>DVM</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="1" t="str">
         <f>Target_Values!B19</f>
-        <v>0</v>
+        <v>Yes</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>34</v>
@@ -1216,25 +1314,26 @@
         <f>Target_Values!A20</f>
         <v>Counter</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="1" t="str">
         <f>Target_Values!B20</f>
-        <v>0</v>
+        <v>Yes</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="str">
         <f>Target_Values!A21</f>
         <v>Besonderheiten</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="6" t="str">
         <f>Target_Values!B21</f>
-        <v>0</v>
-      </c>
-      <c r="C21" s="2" t="s">
+        <v>Bandbreitenupgrade nachträglich möglich
+Optional: Enhanced Security</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D21" s="2"/>
@@ -1244,9 +1343,9 @@
         <f>Target_Values!A22</f>
         <v>Abmessungen (L x B x H) (mm)</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="1" t="str">
         <f>Target_Values!B22</f>
-        <v>0</v>
+        <v>148, 425, 288</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>37</v>
@@ -1260,7 +1359,7 @@
       </c>
       <c r="B23" s="1">
         <f>Target_Values!B23</f>
-        <v>0</v>
+        <v>6.8</v>
       </c>
       <c r="C23" s="2">
         <v>6.8</v>
@@ -1274,7 +1373,7 @@
       </c>
       <c r="B24" s="1">
         <f>Target_Values!B24</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1284,9 +1383,9 @@
         <f>Target_Values!A25</f>
         <v>Artikelnummer</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="1" t="str">
         <f>Target_Values!B25</f>
-        <v>0</v>
+        <v>DSOX6004A</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>26</v>
@@ -1336,9 +1435,9 @@
         <f>Target_Values!A2</f>
         <v>Modell</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="1" t="str">
         <f>Target_Values!B2</f>
-        <v>0</v>
+        <v>DSOX6004A</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1348,7 +1447,7 @@
       </c>
       <c r="B3" s="1">
         <f>Target_Values!B3</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1358,7 +1457,7 @@
       </c>
       <c r="B4" s="1">
         <f>Target_Values!B4</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1368,7 +1467,7 @@
       </c>
       <c r="B5" s="1">
         <f>Target_Values!B5</f>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1378,7 +1477,7 @@
       </c>
       <c r="B6" s="1">
         <f>Target_Values!B6</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1386,9 +1485,10 @@
         <f>Target_Values!A7</f>
         <v>Triggerarten</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="1" t="str">
         <f>Target_Values!B7</f>
-        <v>0</v>
+        <v>Zone (hardware zone qualifier), Edge, Edge then edge (B trigger), Pulse width, Pattern, Or, Rise/fall time, Nth edge burst, Runt, Setup and hold, Video
+Optional: Enhanced video</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1398,7 +1498,7 @@
       </c>
       <c r="B8" s="1">
         <f>Target_Values!B8</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1418,7 +1518,7 @@
       </c>
       <c r="B10" s="1">
         <f>Target_Values!B10</f>
-        <v>0</v>
+        <v>30.7</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1426,9 +1526,9 @@
         <f>Target_Values!A11</f>
         <v>Bildschirmtyp.pixel</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="1" t="str">
         <f>Target_Values!B11</f>
-        <v>0</v>
+        <v>800, 600</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1436,9 +1536,9 @@
         <f>Target_Values!A12</f>
         <v>Bildschirmtyp.screen_type</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="1" t="str">
         <f>Target_Values!B12</f>
-        <v>0</v>
+        <v>Touchscreen</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1446,9 +1546,9 @@
         <f>Target_Values!A13</f>
         <v>Schnittstellen.relevant_interfaces</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="1" t="str">
         <f>Target_Values!B13</f>
-        <v>0</v>
+        <v>USB, LAN</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1456,9 +1556,9 @@
         <f>Target_Values!A14</f>
         <v>Schnittstellen.optionale_interfaces</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="1" t="str">
         <f>Target_Values!B14</f>
-        <v>0</v>
+        <v>GPIB</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1466,9 +1566,9 @@
         <f>Target_Values!A15</f>
         <v>unterstützende serielle Busse</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="1" t="str">
         <f>Target_Values!B15</f>
-        <v>0</v>
+        <v>Optional: ARINC429, CAN, FlexRay, I²C, I²S, LIN, MIL-STD1553, SPI, UART/RS232/422/485, USB, SENT, User-definable Manchester/NRZ, CXPI, USB PD</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1478,7 +1578,7 @@
       </c>
       <c r="B16" s="1">
         <f>Target_Values!B16</f>
-        <v>0</v>
+        <v>450000</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1486,9 +1586,9 @@
         <f>Target_Values!A17</f>
         <v>segmentierbarer Speicher</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="1" t="str">
         <f>Target_Values!B17</f>
-        <v>0</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1496,9 +1596,9 @@
         <f>Target_Values!A18</f>
         <v>Funktionsgenerator</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="1" t="str">
         <f>Target_Values!B18</f>
-        <v>0</v>
+        <v>Optional</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1506,9 +1606,9 @@
         <f>Target_Values!A19</f>
         <v>DVM</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="1" t="str">
         <f>Target_Values!B19</f>
-        <v>0</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1516,9 +1616,9 @@
         <f>Target_Values!A20</f>
         <v>Counter</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="1" t="str">
         <f>Target_Values!B20</f>
-        <v>0</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1526,9 +1626,10 @@
         <f>Target_Values!A21</f>
         <v>Besonderheiten</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="1" t="str">
         <f>Target_Values!B21</f>
-        <v>0</v>
+        <v>Bandbreitenupgrade nachträglich möglich
+Optional: Enhanced Security</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1536,9 +1637,9 @@
         <f>Target_Values!A22</f>
         <v>Abmessungen (L x B x H) (mm)</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="1" t="str">
         <f>Target_Values!B22</f>
-        <v>0</v>
+        <v>148, 425, 288</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1548,7 +1649,7 @@
       </c>
       <c r="B23" s="1">
         <f>Target_Values!B23</f>
-        <v>0</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1558,7 +1659,7 @@
       </c>
       <c r="B24" s="1">
         <f>Target_Values!B24</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1566,9 +1667,9 @@
         <f>Target_Values!A25</f>
         <v>Artikelnummer</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="1" t="str">
         <f>Target_Values!B25</f>
-        <v>0</v>
+        <v>DSOX6004A</v>
       </c>
     </row>
   </sheetData>
@@ -1608,9 +1709,9 @@
         <f>Target_Values!A2</f>
         <v>Modell</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="1" t="str">
         <f>Target_Values!B2</f>
-        <v>0</v>
+        <v>DSOX6004A</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1620,7 +1721,7 @@
       </c>
       <c r="B3" s="1">
         <f>Target_Values!B3</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1630,7 +1731,7 @@
       </c>
       <c r="B4" s="1">
         <f>Target_Values!B4</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1640,7 +1741,7 @@
       </c>
       <c r="B5" s="1">
         <f>Target_Values!B5</f>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1650,7 +1751,7 @@
       </c>
       <c r="B6" s="1">
         <f>Target_Values!B6</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1658,9 +1759,10 @@
         <f>Target_Values!A7</f>
         <v>Triggerarten</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="1" t="str">
         <f>Target_Values!B7</f>
-        <v>0</v>
+        <v>Zone (hardware zone qualifier), Edge, Edge then edge (B trigger), Pulse width, Pattern, Or, Rise/fall time, Nth edge burst, Runt, Setup and hold, Video
+Optional: Enhanced video</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1670,7 +1772,7 @@
       </c>
       <c r="B8" s="1">
         <f>Target_Values!B8</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1690,7 +1792,7 @@
       </c>
       <c r="B10" s="1">
         <f>Target_Values!B10</f>
-        <v>0</v>
+        <v>30.7</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1698,9 +1800,9 @@
         <f>Target_Values!A11</f>
         <v>Bildschirmtyp.pixel</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="1" t="str">
         <f>Target_Values!B11</f>
-        <v>0</v>
+        <v>800, 600</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1708,9 +1810,9 @@
         <f>Target_Values!A12</f>
         <v>Bildschirmtyp.screen_type</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="1" t="str">
         <f>Target_Values!B12</f>
-        <v>0</v>
+        <v>Touchscreen</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1718,9 +1820,9 @@
         <f>Target_Values!A13</f>
         <v>Schnittstellen.relevant_interfaces</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="1" t="str">
         <f>Target_Values!B13</f>
-        <v>0</v>
+        <v>USB, LAN</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1728,9 +1830,9 @@
         <f>Target_Values!A14</f>
         <v>Schnittstellen.optionale_interfaces</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="1" t="str">
         <f>Target_Values!B14</f>
-        <v>0</v>
+        <v>GPIB</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1738,9 +1840,9 @@
         <f>Target_Values!A15</f>
         <v>unterstützende serielle Busse</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="1" t="str">
         <f>Target_Values!B15</f>
-        <v>0</v>
+        <v>Optional: ARINC429, CAN, FlexRay, I²C, I²S, LIN, MIL-STD1553, SPI, UART/RS232/422/485, USB, SENT, User-definable Manchester/NRZ, CXPI, USB PD</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1750,7 +1852,7 @@
       </c>
       <c r="B16" s="1">
         <f>Target_Values!B16</f>
-        <v>0</v>
+        <v>450000</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1758,9 +1860,9 @@
         <f>Target_Values!A17</f>
         <v>segmentierbarer Speicher</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="1" t="str">
         <f>Target_Values!B17</f>
-        <v>0</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1768,9 +1870,9 @@
         <f>Target_Values!A18</f>
         <v>Funktionsgenerator</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="1" t="str">
         <f>Target_Values!B18</f>
-        <v>0</v>
+        <v>Optional</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1778,9 +1880,9 @@
         <f>Target_Values!A19</f>
         <v>DVM</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="1" t="str">
         <f>Target_Values!B19</f>
-        <v>0</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1788,9 +1890,9 @@
         <f>Target_Values!A20</f>
         <v>Counter</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="1" t="str">
         <f>Target_Values!B20</f>
-        <v>0</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1798,9 +1900,10 @@
         <f>Target_Values!A21</f>
         <v>Besonderheiten</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="1" t="str">
         <f>Target_Values!B21</f>
-        <v>0</v>
+        <v>Bandbreitenupgrade nachträglich möglich
+Optional: Enhanced Security</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1808,9 +1911,9 @@
         <f>Target_Values!A22</f>
         <v>Abmessungen (L x B x H) (mm)</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="1" t="str">
         <f>Target_Values!B22</f>
-        <v>0</v>
+        <v>148, 425, 288</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1820,7 +1923,7 @@
       </c>
       <c r="B23" s="1">
         <f>Target_Values!B23</f>
-        <v>0</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1830,7 +1933,7 @@
       </c>
       <c r="B24" s="1">
         <f>Target_Values!B24</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1838,9 +1941,9 @@
         <f>Target_Values!A25</f>
         <v>Artikelnummer</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="1" t="str">
         <f>Target_Values!B25</f>
-        <v>0</v>
+        <v>DSOX6004A</v>
       </c>
     </row>
   </sheetData>
@@ -1880,9 +1983,9 @@
         <f>Target_Values!A2</f>
         <v>Modell</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="1" t="str">
         <f>Target_Values!B2</f>
-        <v>0</v>
+        <v>DSOX6004A</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1892,7 +1995,7 @@
       </c>
       <c r="B3" s="1">
         <f>Target_Values!B3</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1902,7 +2005,7 @@
       </c>
       <c r="B4" s="1">
         <f>Target_Values!B4</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1912,7 +2015,7 @@
       </c>
       <c r="B5" s="1">
         <f>Target_Values!B5</f>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1922,7 +2025,7 @@
       </c>
       <c r="B6" s="1">
         <f>Target_Values!B6</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1930,9 +2033,10 @@
         <f>Target_Values!A7</f>
         <v>Triggerarten</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="1" t="str">
         <f>Target_Values!B7</f>
-        <v>0</v>
+        <v>Zone (hardware zone qualifier), Edge, Edge then edge (B trigger), Pulse width, Pattern, Or, Rise/fall time, Nth edge burst, Runt, Setup and hold, Video
+Optional: Enhanced video</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1942,7 +2046,7 @@
       </c>
       <c r="B8" s="1">
         <f>Target_Values!B8</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1962,7 +2066,7 @@
       </c>
       <c r="B10" s="1">
         <f>Target_Values!B10</f>
-        <v>0</v>
+        <v>30.7</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1970,9 +2074,9 @@
         <f>Target_Values!A11</f>
         <v>Bildschirmtyp.pixel</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="1" t="str">
         <f>Target_Values!B11</f>
-        <v>0</v>
+        <v>800, 600</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1980,9 +2084,9 @@
         <f>Target_Values!A12</f>
         <v>Bildschirmtyp.screen_type</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="1" t="str">
         <f>Target_Values!B12</f>
-        <v>0</v>
+        <v>Touchscreen</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1990,9 +2094,9 @@
         <f>Target_Values!A13</f>
         <v>Schnittstellen.relevant_interfaces</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="1" t="str">
         <f>Target_Values!B13</f>
-        <v>0</v>
+        <v>USB, LAN</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2000,9 +2104,9 @@
         <f>Target_Values!A14</f>
         <v>Schnittstellen.optionale_interfaces</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="1" t="str">
         <f>Target_Values!B14</f>
-        <v>0</v>
+        <v>GPIB</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2010,9 +2114,9 @@
         <f>Target_Values!A15</f>
         <v>unterstützende serielle Busse</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="1" t="str">
         <f>Target_Values!B15</f>
-        <v>0</v>
+        <v>Optional: ARINC429, CAN, FlexRay, I²C, I²S, LIN, MIL-STD1553, SPI, UART/RS232/422/485, USB, SENT, User-definable Manchester/NRZ, CXPI, USB PD</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2022,7 +2126,7 @@
       </c>
       <c r="B16" s="1">
         <f>Target_Values!B16</f>
-        <v>0</v>
+        <v>450000</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2030,9 +2134,9 @@
         <f>Target_Values!A17</f>
         <v>segmentierbarer Speicher</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="1" t="str">
         <f>Target_Values!B17</f>
-        <v>0</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2040,9 +2144,9 @@
         <f>Target_Values!A18</f>
         <v>Funktionsgenerator</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="1" t="str">
         <f>Target_Values!B18</f>
-        <v>0</v>
+        <v>Optional</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2050,9 +2154,9 @@
         <f>Target_Values!A19</f>
         <v>DVM</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="1" t="str">
         <f>Target_Values!B19</f>
-        <v>0</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2060,9 +2164,9 @@
         <f>Target_Values!A20</f>
         <v>Counter</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="1" t="str">
         <f>Target_Values!B20</f>
-        <v>0</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2070,9 +2174,10 @@
         <f>Target_Values!A21</f>
         <v>Besonderheiten</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="1" t="str">
         <f>Target_Values!B21</f>
-        <v>0</v>
+        <v>Bandbreitenupgrade nachträglich möglich
+Optional: Enhanced Security</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2080,9 +2185,9 @@
         <f>Target_Values!A22</f>
         <v>Abmessungen (L x B x H) (mm)</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="1" t="str">
         <f>Target_Values!B22</f>
-        <v>0</v>
+        <v>148, 425, 288</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2092,7 +2197,7 @@
       </c>
       <c r="B23" s="1">
         <f>Target_Values!B23</f>
-        <v>0</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2102,7 +2207,7 @@
       </c>
       <c r="B24" s="1">
         <f>Target_Values!B24</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2110,9 +2215,9 @@
         <f>Target_Values!A25</f>
         <v>Artikelnummer</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="1" t="str">
         <f>Target_Values!B25</f>
-        <v>0</v>
+        <v>DSOX6004A</v>
       </c>
     </row>
   </sheetData>
@@ -2152,9 +2257,9 @@
         <f>Target_Values!A2</f>
         <v>Modell</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="1" t="str">
         <f>Target_Values!B2</f>
-        <v>0</v>
+        <v>DSOX6004A</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2164,7 +2269,7 @@
       </c>
       <c r="B3" s="1">
         <f>Target_Values!B3</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2174,7 +2279,7 @@
       </c>
       <c r="B4" s="1">
         <f>Target_Values!B4</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2184,7 +2289,7 @@
       </c>
       <c r="B5" s="1">
         <f>Target_Values!B5</f>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2194,7 +2299,7 @@
       </c>
       <c r="B6" s="1">
         <f>Target_Values!B6</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2202,9 +2307,10 @@
         <f>Target_Values!A7</f>
         <v>Triggerarten</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="1" t="str">
         <f>Target_Values!B7</f>
-        <v>0</v>
+        <v>Zone (hardware zone qualifier), Edge, Edge then edge (B trigger), Pulse width, Pattern, Or, Rise/fall time, Nth edge burst, Runt, Setup and hold, Video
+Optional: Enhanced video</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2214,7 +2320,7 @@
       </c>
       <c r="B8" s="1">
         <f>Target_Values!B8</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2234,7 +2340,7 @@
       </c>
       <c r="B10" s="1">
         <f>Target_Values!B10</f>
-        <v>0</v>
+        <v>30.7</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2242,9 +2348,9 @@
         <f>Target_Values!A11</f>
         <v>Bildschirmtyp.pixel</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="1" t="str">
         <f>Target_Values!B11</f>
-        <v>0</v>
+        <v>800, 600</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2252,9 +2358,9 @@
         <f>Target_Values!A12</f>
         <v>Bildschirmtyp.screen_type</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="1" t="str">
         <f>Target_Values!B12</f>
-        <v>0</v>
+        <v>Touchscreen</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2262,9 +2368,9 @@
         <f>Target_Values!A13</f>
         <v>Schnittstellen.relevant_interfaces</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="1" t="str">
         <f>Target_Values!B13</f>
-        <v>0</v>
+        <v>USB, LAN</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2272,9 +2378,9 @@
         <f>Target_Values!A14</f>
         <v>Schnittstellen.optionale_interfaces</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="1" t="str">
         <f>Target_Values!B14</f>
-        <v>0</v>
+        <v>GPIB</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2282,9 +2388,9 @@
         <f>Target_Values!A15</f>
         <v>unterstützende serielle Busse</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="1" t="str">
         <f>Target_Values!B15</f>
-        <v>0</v>
+        <v>Optional: ARINC429, CAN, FlexRay, I²C, I²S, LIN, MIL-STD1553, SPI, UART/RS232/422/485, USB, SENT, User-definable Manchester/NRZ, CXPI, USB PD</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2294,7 +2400,7 @@
       </c>
       <c r="B16" s="1">
         <f>Target_Values!B16</f>
-        <v>0</v>
+        <v>450000</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2302,9 +2408,9 @@
         <f>Target_Values!A17</f>
         <v>segmentierbarer Speicher</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="1" t="str">
         <f>Target_Values!B17</f>
-        <v>0</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2312,9 +2418,9 @@
         <f>Target_Values!A18</f>
         <v>Funktionsgenerator</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="1" t="str">
         <f>Target_Values!B18</f>
-        <v>0</v>
+        <v>Optional</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2322,9 +2428,9 @@
         <f>Target_Values!A19</f>
         <v>DVM</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="1" t="str">
         <f>Target_Values!B19</f>
-        <v>0</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2332,9 +2438,9 @@
         <f>Target_Values!A20</f>
         <v>Counter</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="1" t="str">
         <f>Target_Values!B20</f>
-        <v>0</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2342,9 +2448,10 @@
         <f>Target_Values!A21</f>
         <v>Besonderheiten</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="1" t="str">
         <f>Target_Values!B21</f>
-        <v>0</v>
+        <v>Bandbreitenupgrade nachträglich möglich
+Optional: Enhanced Security</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2352,9 +2459,9 @@
         <f>Target_Values!A22</f>
         <v>Abmessungen (L x B x H) (mm)</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="1" t="str">
         <f>Target_Values!B22</f>
-        <v>0</v>
+        <v>148, 425, 288</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2364,7 +2471,7 @@
       </c>
       <c r="B23" s="1">
         <f>Target_Values!B23</f>
-        <v>0</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2374,7 +2481,7 @@
       </c>
       <c r="B24" s="1">
         <f>Target_Values!B24</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2382,9 +2489,9 @@
         <f>Target_Values!A25</f>
         <v>Artikelnummer</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="1" t="str">
         <f>Target_Values!B25</f>
-        <v>0</v>
+        <v>DSOX6004A</v>
       </c>
     </row>
   </sheetData>

</xml_diff>